<commit_message>
- slide eklendi - hata azaltıldı
</commit_message>
<xml_diff>
--- a/docs/todo.xlsx
+++ b/docs/todo.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{2CC552C2-D91D-4E71-A0D6-789C004CC786}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{00934CC6-519C-497E-8ED8-FE3498CAD8E4}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>WEB İLE</t>
   </si>
@@ -68,14 +68,46 @@
   </si>
   <si>
     <t>hmtl 5 banner</t>
+  </si>
+  <si>
+    <t>CRON JOB</t>
+  </si>
+  <si>
+    <t>HATA SISTEMI</t>
+  </si>
+  <si>
+    <t>POSITON BULUP GUNCELLEME ( CACHE ALININCA :)</t>
+  </si>
+  <si>
+    <t>tarih null dönme hatası ( boş yap )</t>
+  </si>
+  <si>
+    <t>Önerilenlere id verme</t>
+  </si>
+  <si>
+    <t>Girişte banner ( splash screen )</t>
+  </si>
+  <si>
+    <t>KURUM MOIL APP MAKALE SİTE İÇİN</t>
+  </si>
+  <si>
+    <t>Slider</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -103,9 +135,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -388,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -409,7 +444,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -425,7 +460,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -433,7 +468,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -453,22 +488,55 @@
         <v>12</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="C9" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="C10" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="C11" s="1" t="s">
         <v>15</v>
       </c>
     </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C14" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
- slide eklendi - hata azaltıldı - Update denendi - default db güncellendi
</commit_message>
<xml_diff>
--- a/docs/todo.xlsx
+++ b/docs/todo.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{00934CC6-519C-497E-8ED8-FE3498CAD8E4}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C3E382AE-FE83-4025-AA9E-A3D4324E067B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -426,7 +426,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,7 +447,7 @@
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -455,7 +455,7 @@
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -463,7 +463,7 @@
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -484,12 +484,12 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -510,7 +510,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C11" s="1" t="s">

</xml_diff>